<commit_message>
Final changes in Stock
</commit_message>
<xml_diff>
--- a/ExcelFiles/StockDomain.xlsx
+++ b/ExcelFiles/StockDomain.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4Automation\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA376AF-48DE-41ED-B767-C50E5A3B7B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8650DDAE-88DD-4F80-A77F-62D6D023D0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -296,10 +296,10 @@
     <t>decrement</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>AFUTablet</t>
+    <t>8</t>
+  </si>
+  <si>
+    <t>MedOne</t>
   </si>
 </sst>
 </file>
@@ -1021,7 +1021,7 @@
     <row r="2" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="str">
         <f>AddNewStock!A2</f>
-        <v>AFUTablet</v>
+        <v>MedOne</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -1274,7 +1274,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Push excel for user
</commit_message>
<xml_diff>
--- a/ExcelFiles/StockDomain.xlsx
+++ b/ExcelFiles/StockDomain.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Release_Server\Cellma4Automation\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218EF2BB-EE28-44C8-B58C-5A124156DEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C316B767-F45A-4936-8999-558358862FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="1" r:id="rId1"/>
@@ -743,7 +743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6834B6FC-CAD9-422A-8F3B-C1D76C190C8D}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -921,7 +921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F2A331-EEA0-4CAD-9DF4-CCAD2BA390DC}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>